<commit_message>
Add test case for holding with high ranking parcel in quickly filled bucket
</commit_message>
<xml_diff>
--- a/iacs_qa/BEFL/data/sim_4P_2024_MT.xlsx
+++ b/iacs_qa/BEFL/data/sim_4P_2024_MT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="13">
   <si>
     <t>bucket</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>ranking</t>
+  </si>
+  <si>
+    <t>UA5</t>
   </si>
   <si>
     <t>UA3</t>
@@ -407,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,16 +441,16 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>601</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
       </c>
       <c r="F2">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -458,16 +461,16 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>2195</v>
+        <v>7723</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
       <c r="F3">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -478,16 +481,16 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>7723</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -495,19 +498,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>3289</v>
+        <v>988</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -518,7 +521,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>601</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -527,7 +530,7 @@
         <v>6</v>
       </c>
       <c r="F6">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -538,16 +541,16 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>988</v>
+        <v>2195</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
       <c r="F7">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -555,19 +558,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>6235</v>
+        <v>7723</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -578,16 +581,16 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>75</v>
+        <v>3289</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -598,16 +601,16 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>753</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
       </c>
       <c r="F10">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -618,16 +621,16 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <v>7723</v>
+        <v>988</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -638,16 +641,16 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <v>75</v>
+        <v>6235</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -658,16 +661,16 @@
         <v>8</v>
       </c>
       <c r="C13">
-        <v>2195</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
       </c>
       <c r="F13">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -678,7 +681,7 @@
         <v>8</v>
       </c>
       <c r="C14">
-        <v>1194</v>
+        <v>753</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -687,7 +690,7 @@
         <v>8</v>
       </c>
       <c r="F14">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -698,16 +701,96 @@
         <v>8</v>
       </c>
       <c r="C15">
+        <v>7723</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>2195</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>1194</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19">
         <v>3289</v>
       </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15">
-        <v>7</v>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>